<commit_message>
create .xlsx-df with only log rt
</commit_message>
<xml_diff>
--- a/RData/data_rt_cond.xlsx
+++ b/RData/data_rt_cond.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -375,20 +375,10 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>FPM</t>
+          <t>WPM_log</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>WPM</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>WPM_log</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>FPM_log</t>
         </is>
@@ -407,15 +397,9 @@
         <v>823.4285714285714</v>
       </c>
       <c r="D2">
-        <v>1127.17094017094</v>
+        <v>6.868175328897202</v>
       </c>
       <c r="E2">
-        <v>961.1931034482759</v>
-      </c>
-      <c r="F2">
-        <v>6.868175328897202</v>
-      </c>
-      <c r="G2">
         <v>7.027466179708268</v>
       </c>
     </row>
@@ -432,15 +416,9 @@
         <v>185.2857142857143</v>
       </c>
       <c r="D3">
-        <v>1675.709090909091</v>
+        <v>7.235590887291337</v>
       </c>
       <c r="E3">
-        <v>1387.960784313726</v>
-      </c>
-      <c r="F3">
-        <v>7.235590887291337</v>
-      </c>
-      <c r="G3">
         <v>7.423991692533152</v>
       </c>
     </row>
@@ -457,15 +435,9 @@
         <v>280.8571428571428</v>
       </c>
       <c r="D4">
-        <v>1313.71724137931</v>
+        <v>6.897691652237548</v>
       </c>
       <c r="E4">
-        <v>989.9868421052631</v>
-      </c>
-      <c r="F4">
-        <v>6.897691652237548</v>
-      </c>
-      <c r="G4">
         <v>7.180615986678988</v>
       </c>
     </row>
@@ -482,15 +454,9 @@
         <v>334.4285714285714</v>
       </c>
       <c r="D5">
-        <v>1330.225806451613</v>
+        <v>7.271008538280992</v>
       </c>
       <c r="E5">
-        <v>1438</v>
-      </c>
-      <c r="F5">
-        <v>7.271008538280992</v>
-      </c>
-      <c r="G5">
         <v>7.193103986091854</v>
       </c>
     </row>
@@ -507,15 +473,9 @@
         <v>509.2857142857143</v>
       </c>
       <c r="D6">
-        <v>1327.21568627451</v>
+        <v>6.938973119086882</v>
       </c>
       <c r="E6">
-        <v>1031.710227272727</v>
-      </c>
-      <c r="F6">
-        <v>6.938973119086882</v>
-      </c>
-      <c r="G6">
         <v>7.190838557880011</v>
       </c>
     </row>
@@ -532,15 +492,9 @@
         <v>516.8571428571429</v>
       </c>
       <c r="D7">
-        <v>1466.961038961039</v>
+        <v>6.869672146386769</v>
       </c>
       <c r="E7">
-        <v>962.632911392405</v>
-      </c>
-      <c r="F7">
-        <v>6.869672146386769</v>
-      </c>
-      <c r="G7">
         <v>7.290948219481536</v>
       </c>
     </row>
@@ -557,15 +511,9 @@
         <v>337.2857142857143</v>
       </c>
       <c r="D8">
-        <v>1162.716981132075</v>
+        <v>6.765143826059799</v>
       </c>
       <c r="E8">
-        <v>867.0909090909091</v>
-      </c>
-      <c r="F8">
-        <v>6.765143826059799</v>
-      </c>
-      <c r="G8">
         <v>7.05851477048068</v>
       </c>
     </row>
@@ -582,15 +530,9 @@
         <v>469.2857142857143</v>
       </c>
       <c r="D9">
-        <v>2181.214285714286</v>
+        <v>7.521484556637388</v>
       </c>
       <c r="E9">
-        <v>1847.307692307692</v>
-      </c>
-      <c r="F9">
-        <v>7.521484556637388</v>
-      </c>
-      <c r="G9">
         <v>7.687637012505191</v>
       </c>
     </row>
@@ -607,15 +549,9 @@
         <v>31.28571428571428</v>
       </c>
       <c r="D10">
-        <v>1369.927083333333</v>
+        <v>7.07880722235384</v>
       </c>
       <c r="E10">
-        <v>1186.552380952381</v>
-      </c>
-      <c r="F10">
-        <v>7.07880722235384</v>
-      </c>
-      <c r="G10">
         <v>7.222512793561449</v>
       </c>
     </row>
@@ -632,15 +568,9 @@
         <v>331.1428571428572</v>
       </c>
       <c r="D11">
-        <v>1311.64705882353</v>
+        <v>6.921752746160236</v>
       </c>
       <c r="E11">
-        <v>1014.095890410959</v>
-      </c>
-      <c r="F11">
-        <v>6.921752746160236</v>
-      </c>
-      <c r="G11">
         <v>7.179038923271301</v>
       </c>
     </row>
@@ -657,15 +587,9 @@
         <v>1422.428571428571</v>
       </c>
       <c r="D12">
-        <v>1851.617391304348</v>
+        <v>7.28302250744285</v>
       </c>
       <c r="E12">
-        <v>1455.380281690141</v>
-      </c>
-      <c r="F12">
-        <v>7.28302250744285</v>
-      </c>
-      <c r="G12">
         <v>7.523814801694744</v>
       </c>
     </row>
@@ -682,15 +606,9 @@
         <v>239.7142857142857</v>
       </c>
       <c r="D13">
-        <v>1469.75</v>
+        <v>7.343147902864423</v>
       </c>
       <c r="E13">
-        <v>1545.56976744186</v>
-      </c>
-      <c r="F13">
-        <v>7.343147902864423</v>
-      </c>
-      <c r="G13">
         <v>7.292847597282364</v>
       </c>
     </row>
@@ -707,15 +625,9 @@
         <v>450.8571428571428</v>
       </c>
       <c r="D14">
-        <v>1101.44512195122</v>
+        <v>6.754401649846619</v>
       </c>
       <c r="E14">
-        <v>857.8263157894737</v>
-      </c>
-      <c r="F14">
-        <v>6.754401649846619</v>
-      </c>
-      <c r="G14">
         <v>7.004378343804022</v>
       </c>
     </row>
@@ -732,15 +644,9 @@
         <v>443.1428571428572</v>
       </c>
       <c r="D15">
-        <v>1357.531914893617</v>
+        <v>6.945890590677042</v>
       </c>
       <c r="E15">
-        <v>1038.871794871795</v>
-      </c>
-      <c r="F15">
-        <v>6.945890590677042</v>
-      </c>
-      <c r="G15">
         <v>7.21342356158228</v>
       </c>
     </row>
@@ -757,15 +663,9 @@
         <v>405.5714285714286</v>
       </c>
       <c r="D16">
-        <v>1152.467625899281</v>
+        <v>6.680493671059009</v>
       </c>
       <c r="E16">
-        <v>796.7123287671233</v>
-      </c>
-      <c r="F16">
-        <v>6.680493671059009</v>
-      </c>
-      <c r="G16">
         <v>7.049660684150259</v>
       </c>
     </row>
@@ -782,15 +682,9 @@
         <v>179.8571428571429</v>
       </c>
       <c r="D17">
-        <v>1425.090909090909</v>
+        <v>6.903808105191785</v>
       </c>
       <c r="E17">
-        <v>996.060606060606</v>
-      </c>
-      <c r="F17">
-        <v>6.903808105191785</v>
-      </c>
-      <c r="G17">
         <v>7.261990886521152</v>
       </c>
     </row>
@@ -807,15 +701,9 @@
         <v>202.7142857142857</v>
       </c>
       <c r="D18">
-        <v>1789.952380952381</v>
+        <v>7.288239991158792</v>
       </c>
       <c r="E18">
-        <v>1462.993548387097</v>
-      </c>
-      <c r="F18">
-        <v>7.288239991158792</v>
-      </c>
-      <c r="G18">
         <v>7.489944295661041</v>
       </c>
     </row>
@@ -832,15 +720,9 @@
         <v>141.7142857142857</v>
       </c>
       <c r="D19">
-        <v>2100.153846153846</v>
+        <v>7.364293657274302</v>
       </c>
       <c r="E19">
-        <v>1578.6</v>
-      </c>
-      <c r="F19">
-        <v>7.364293657274302</v>
-      </c>
-      <c r="G19">
         <v>7.649765881101386</v>
       </c>
     </row>
@@ -857,15 +739,9 @@
         <v>275</v>
       </c>
       <c r="D20">
-        <v>1302.801369863014</v>
+        <v>6.952684029225537</v>
       </c>
       <c r="E20">
-        <v>1045.953333333333</v>
-      </c>
-      <c r="F20">
-        <v>6.952684029225537</v>
-      </c>
-      <c r="G20">
         <v>7.172272124877588</v>
       </c>
     </row>
@@ -882,15 +758,9 @@
         <v>555.8571428571429</v>
       </c>
       <c r="D21">
-        <v>1223.923076923077</v>
+        <v>6.689054966844467</v>
       </c>
       <c r="E21">
-        <v>803.5625</v>
-      </c>
-      <c r="F21">
-        <v>6.689054966844467</v>
-      </c>
-      <c r="G21">
         <v>7.10981661544632</v>
       </c>
     </row>
@@ -907,15 +777,9 @@
         <v>843.2857142857143</v>
       </c>
       <c r="D22">
-        <v>1638.9</v>
+        <v>7.145163944947113</v>
       </c>
       <c r="E22">
-        <v>1267.959183673469</v>
-      </c>
-      <c r="F22">
-        <v>7.145163944947113</v>
-      </c>
-      <c r="G22">
         <v>7.401780564069782</v>
       </c>
     </row>
@@ -932,15 +796,9 @@
         <v>146.2857142857143</v>
       </c>
       <c r="D23">
-        <v>1549.987654320988</v>
+        <v>7.105047066617693</v>
       </c>
       <c r="E23">
-        <v>1218.099415204678</v>
-      </c>
-      <c r="F23">
-        <v>7.105047066617693</v>
-      </c>
-      <c r="G23">
         <v>7.34600224492737</v>
       </c>
     </row>
@@ -957,15 +815,9 @@
         <v>162.2857142857143</v>
       </c>
       <c r="D24">
-        <v>969.2132352941177</v>
+        <v>6.724701539314093</v>
       </c>
       <c r="E24">
-        <v>832.7234042553191</v>
-      </c>
-      <c r="F24">
-        <v>6.724701539314093</v>
-      </c>
-      <c r="G24">
         <v>6.876484644744835</v>
       </c>
     </row>
@@ -982,15 +834,9 @@
         <v>481.5714285714286</v>
       </c>
       <c r="D25">
-        <v>1165.78021978022</v>
+        <v>7.014093534318485</v>
       </c>
       <c r="E25">
-        <v>1112.19801980198</v>
-      </c>
-      <c r="F25">
-        <v>7.014093534318485</v>
-      </c>
-      <c r="G25">
         <v>7.061145858389295</v>
       </c>
     </row>
@@ -1007,15 +853,9 @@
         <v>128.5714285714286</v>
       </c>
       <c r="D26">
-        <v>1225.128</v>
+        <v>6.906132341109006</v>
       </c>
       <c r="E26">
-        <v>998.3783783783783</v>
-      </c>
-      <c r="F26">
-        <v>6.906132341109006</v>
-      </c>
-      <c r="G26">
         <v>7.110800607316067</v>
       </c>
     </row>
@@ -1032,15 +872,9 @@
         <v>131.4285714285714</v>
       </c>
       <c r="D27">
-        <v>799.9130434782609</v>
+        <v>6.389721196913212</v>
       </c>
       <c r="E27">
-        <v>595.6904761904761</v>
-      </c>
-      <c r="F27">
-        <v>6.389721196913212</v>
-      </c>
-      <c r="G27">
         <v>6.684503026107953</v>
       </c>
     </row>
@@ -1057,15 +891,9 @@
         <v>436.4285714285714</v>
       </c>
       <c r="D28">
-        <v>1278.203389830509</v>
+        <v>6.976161311646197</v>
       </c>
       <c r="E28">
-        <v>1070.8</v>
-      </c>
-      <c r="F28">
-        <v>6.976161311646197</v>
-      </c>
-      <c r="G28">
         <v>7.153210769247173</v>
       </c>
     </row>
@@ -1082,15 +910,9 @@
         <v>121.5714285714286</v>
       </c>
       <c r="D29">
-        <v>886.3728813559322</v>
+        <v>6.529226008764224</v>
       </c>
       <c r="E29">
-        <v>684.8679245283018</v>
-      </c>
-      <c r="F29">
-        <v>6.529226008764224</v>
-      </c>
-      <c r="G29">
         <v>6.787137721386846</v>
       </c>
     </row>
@@ -1107,15 +929,9 @@
         <v>308</v>
       </c>
       <c r="D30">
-        <v>1371.18320610687</v>
+        <v>6.952293994294211</v>
       </c>
       <c r="E30">
-        <v>1045.545454545455</v>
-      </c>
-      <c r="F30">
-        <v>6.952293994294211</v>
-      </c>
-      <c r="G30">
         <v>7.223429300180174</v>
       </c>
     </row>
@@ -1132,15 +948,9 @@
         <v>96.71428571428571</v>
       </c>
       <c r="D31">
-        <v>1235.730434782609</v>
+        <v>6.969570368381352</v>
       </c>
       <c r="E31">
-        <v>1063.765625</v>
-      </c>
-      <c r="F31">
-        <v>6.969570368381352</v>
-      </c>
-      <c r="G31">
         <v>7.119417519395422</v>
       </c>
     </row>
@@ -1157,15 +967,9 @@
         <v>107.5714285714286</v>
       </c>
       <c r="D32">
-        <v>1535.657894736842</v>
+        <v>7.235921224281354</v>
       </c>
       <c r="E32">
-        <v>1388.41935483871</v>
-      </c>
-      <c r="F32">
-        <v>7.235921224281354</v>
-      </c>
-      <c r="G32">
         <v>7.336714164120068</v>
       </c>
     </row>
@@ -1182,15 +986,9 @@
         <v>331.5714285714286</v>
       </c>
       <c r="D33">
-        <v>1581.079646017699</v>
+        <v>7.042858499018744</v>
       </c>
       <c r="E33">
-        <v>1144.654929577465</v>
-      </c>
-      <c r="F33">
-        <v>7.042858499018744</v>
-      </c>
-      <c r="G33">
         <v>7.365863212928386</v>
       </c>
     </row>
@@ -1207,15 +1005,9 @@
         <v>161.7142857142857</v>
       </c>
       <c r="D34">
-        <v>1301.338842975207</v>
+        <v>6.879172072121193</v>
       </c>
       <c r="E34">
-        <v>971.8214285714286</v>
-      </c>
-      <c r="F34">
-        <v>6.879172072121193</v>
-      </c>
-      <c r="G34">
         <v>7.171148892699564</v>
       </c>
     </row>
@@ -1232,15 +1024,9 @@
         <v>229.8571428571429</v>
       </c>
       <c r="D35">
-        <v>1375.584745762712</v>
+        <v>6.992008888570469</v>
       </c>
       <c r="E35">
-        <v>1087.904761904762</v>
-      </c>
-      <c r="F35">
-        <v>6.992008888570469</v>
-      </c>
-      <c r="G35">
         <v>7.226634189344773</v>
       </c>
     </row>
@@ -1257,15 +1043,9 @@
         <v>196.7142857142857</v>
       </c>
       <c r="D36">
-        <v>1433.088607594937</v>
+        <v>7.065195922250192</v>
       </c>
       <c r="E36">
-        <v>1170.511278195489</v>
-      </c>
-      <c r="F36">
-        <v>7.065195922250192</v>
-      </c>
-      <c r="G36">
         <v>7.267587259548748</v>
       </c>
     </row>
@@ -1282,15 +1062,9 @@
         <v>390.1428571428572</v>
       </c>
       <c r="D37">
-        <v>1274.812903225806</v>
+        <v>6.856096333132005</v>
       </c>
       <c r="E37">
-        <v>949.6526946107784</v>
-      </c>
-      <c r="F37">
-        <v>6.856096333132005</v>
-      </c>
-      <c r="G37">
         <v>7.150554704256788</v>
       </c>
     </row>
@@ -1307,15 +1081,9 @@
         <v>137.2857142857143</v>
       </c>
       <c r="D38">
-        <v>1127.573529411765</v>
+        <v>6.672539146433658</v>
       </c>
       <c r="E38">
-        <v>790.4</v>
-      </c>
-      <c r="F38">
-        <v>6.672539146433658</v>
-      </c>
-      <c r="G38">
         <v>7.027823283806345</v>
       </c>
     </row>
@@ -1332,15 +1100,9 @@
         <v>1061</v>
       </c>
       <c r="D39">
-        <v>1108.344262295082</v>
+        <v>6.77639296078531</v>
       </c>
       <c r="E39">
-        <v>876.9</v>
-      </c>
-      <c r="F39">
-        <v>6.77639296078531</v>
-      </c>
-      <c r="G39">
         <v>7.010622525090596</v>
       </c>
     </row>
@@ -1357,15 +1119,9 @@
         <v>79.14285714285714</v>
       </c>
       <c r="D40">
-        <v>1588.352459016393</v>
+        <v>7.14185139731475</v>
       </c>
       <c r="E40">
-        <v>1263.765957446808</v>
-      </c>
-      <c r="F40">
-        <v>7.14185139731475</v>
-      </c>
-      <c r="G40">
         <v>7.370452568701144</v>
       </c>
     </row>
@@ -1382,15 +1138,9 @@
         <v>95.85714285714286</v>
       </c>
       <c r="D41">
-        <v>992.7404580152672</v>
+        <v>6.654818846307865</v>
       </c>
       <c r="E41">
-        <v>776.5172413793103</v>
-      </c>
-      <c r="F41">
-        <v>6.654818846307865</v>
-      </c>
-      <c r="G41">
         <v>6.900469258295833</v>
       </c>
     </row>
@@ -1407,15 +1157,9 @@
         <v>78.14285714285714</v>
       </c>
       <c r="D42">
-        <v>1370.915966386555</v>
+        <v>7.134752811483845</v>
       </c>
       <c r="E42">
-        <v>1254.826771653543</v>
-      </c>
-      <c r="F42">
-        <v>7.134752811483845</v>
-      </c>
-      <c r="G42">
         <v>7.223234384019707</v>
       </c>
     </row>
@@ -1432,15 +1176,9 @@
         <v>310.4285714285714</v>
       </c>
       <c r="D43">
-        <v>1064.655405405405</v>
+        <v>6.805950339526814</v>
       </c>
       <c r="E43">
-        <v>903.2057142857143</v>
-      </c>
-      <c r="F43">
-        <v>6.805950339526814</v>
-      </c>
-      <c r="G43">
         <v>6.970406462786104</v>
       </c>
     </row>
@@ -1457,15 +1195,9 @@
         <v>101</v>
       </c>
       <c r="D44">
-        <v>1225.5</v>
+        <v>6.823411103516777</v>
       </c>
       <c r="E44">
-        <v>919.1148648648649</v>
-      </c>
-      <c r="F44">
-        <v>6.823411103516777</v>
-      </c>
-      <c r="G44">
         <v>7.111104202968168</v>
       </c>
     </row>
@@ -1482,15 +1214,9 @@
         <v>123.5714285714286</v>
       </c>
       <c r="D45">
-        <v>908.1098901098901</v>
+        <v>6.574279595328631</v>
       </c>
       <c r="E45">
-        <v>716.4293193717277</v>
-      </c>
-      <c r="F45">
-        <v>6.574279595328631</v>
-      </c>
-      <c r="G45">
         <v>6.811365395628536</v>
       </c>
     </row>
@@ -1507,15 +1233,9 @@
         <v>186.7142857142857</v>
       </c>
       <c r="D46">
-        <v>740.609756097561</v>
+        <v>6.421239602538288</v>
       </c>
       <c r="E46">
-        <v>614.7647058823529</v>
-      </c>
-      <c r="F46">
-        <v>6.421239602538288</v>
-      </c>
-      <c r="G46">
         <v>6.607473841627368</v>
       </c>
     </row>
@@ -1532,15 +1252,9 @@
         <v>89.42857142857143</v>
       </c>
       <c r="D47">
-        <v>1259.735294117647</v>
+        <v>6.961060523195856</v>
       </c>
       <c r="E47">
-        <v>1054.751552795031</v>
-      </c>
-      <c r="F47">
-        <v>6.961060523195856</v>
-      </c>
-      <c r="G47">
         <v>7.138656893841168</v>
       </c>
     </row>
@@ -1557,15 +1271,9 @@
         <v>43.28571428571428</v>
       </c>
       <c r="D48">
-        <v>1191.714285714286</v>
+        <v>6.959349987793811</v>
       </c>
       <c r="E48">
-        <v>1052.948905109489</v>
-      </c>
-      <c r="F48">
-        <v>6.959349987793811</v>
-      </c>
-      <c r="G48">
         <v>7.083148125701578</v>
       </c>
     </row>
@@ -1582,15 +1290,9 @@
         <v>60.42857142857143</v>
       </c>
       <c r="D49">
-        <v>1569.258928571429</v>
+        <v>7.225240799600637</v>
       </c>
       <c r="E49">
-        <v>1373.66935483871</v>
-      </c>
-      <c r="F49">
-        <v>7.225240799600637</v>
-      </c>
-      <c r="G49">
         <v>7.358358766887639</v>
       </c>
     </row>
@@ -1607,15 +1309,9 @@
         <v>34.42857142857143</v>
       </c>
       <c r="D50">
-        <v>1258.352517985611</v>
+        <v>6.858551904453062</v>
       </c>
       <c r="E50">
-        <v>951.9875</v>
-      </c>
-      <c r="F50">
-        <v>6.858551904453062</v>
-      </c>
-      <c r="G50">
         <v>7.137558618980075</v>
       </c>
     </row>
@@ -1632,15 +1328,9 @@
         <v>31.71428571428572</v>
       </c>
       <c r="D51">
-        <v>1806.15</v>
+        <v>7.342688249360188</v>
       </c>
       <c r="E51">
-        <v>1544.859504132231</v>
-      </c>
-      <c r="F51">
-        <v>7.342688249360188</v>
-      </c>
-      <c r="G51">
         <v>7.498952787006337</v>
       </c>
     </row>
@@ -1657,15 +1347,9 @@
         <v>28.71428571428572</v>
       </c>
       <c r="D52">
-        <v>1148.148936170213</v>
+        <v>6.852448473005276</v>
       </c>
       <c r="E52">
-        <v>946.1948051948052</v>
-      </c>
-      <c r="F52">
-        <v>6.852448473005276</v>
-      </c>
-      <c r="G52">
         <v>7.045906303804517</v>
       </c>
     </row>

</xml_diff>